<commit_message>
refactor(cleanup): remove obsolete configuration and script files, including `.ruffignore`, `.type_ignore_baseline.json`, and `concatenate_script.py`. Updated pre-commit configuration and ensured consistent formatting and linting across all modified files.
</commit_message>
<xml_diff>
--- a/examples/scripts/io/adjustments/exported_adjustments.xlsx
+++ b/examples/scripts/io/adjustments/exported_adjustments.xlsx
@@ -541,7 +541,7 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>2456f628-7c9d-4484-8ee0-f53b2a4bd2fe</t>
+          <t>3cac07d0-817c-4bab-a94a-fd2a97672241</t>
         </is>
       </c>
     </row>
@@ -590,7 +590,7 @@
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr">
         <is>
-          <t>1965caaf-0280-4f5b-a551-21636b439f62</t>
+          <t>26f90013-96b9-4131-a247-02c8793686a3</t>
         </is>
       </c>
     </row>

</xml_diff>